<commit_message>
Had to modify a few numbers in Boulder Demand Charge (they were question marks). Also adding Plot_SensiRuns.m (work in progress)
</commit_message>
<xml_diff>
--- a/Model/Sensi Runs/RunCombos.xlsx
+++ b/Model/Sensi Runs/RunCombos.xlsx
@@ -1,21 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Steve Peterson\GitHub\Utility-D-S\Model\Sensi Runs\Master\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="26423"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11835"/>
+    <workbookView xWindow="9060" yWindow="20" windowWidth="19740" windowHeight="16620"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
@@ -1684,7 +1682,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1719,7 +1717,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1896,7 +1894,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1906,13 +1904,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J513"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:J513"/>
+    <sheetView tabSelected="1" topLeftCell="A239" workbookViewId="0">
+      <selection activeCell="B257" sqref="B257"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="2" max="2" width="15.33203125" customWidth="1"/>
+    <col min="3" max="3" width="19" customWidth="1"/>
+    <col min="4" max="4" width="14.33203125" customWidth="1"/>
+    <col min="5" max="5" width="20.6640625" customWidth="1"/>
+    <col min="6" max="6" width="13.6640625" customWidth="1"/>
+    <col min="7" max="7" width="11.6640625" customWidth="1"/>
+    <col min="8" max="8" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.5" customWidth="1"/>
+    <col min="10" max="10" width="11" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -1941,7 +1950,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -1973,7 +1982,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -2005,7 +2014,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -2037,7 +2046,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -2069,7 +2078,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -2101,7 +2110,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -2133,7 +2142,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -2165,7 +2174,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -2197,7 +2206,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -2229,7 +2238,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -2261,7 +2270,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10">
       <c r="A12" t="s">
         <v>19</v>
       </c>
@@ -2293,7 +2302,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10">
       <c r="A13" t="s">
         <v>20</v>
       </c>
@@ -2325,7 +2334,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10">
       <c r="A14" t="s">
         <v>21</v>
       </c>
@@ -2357,7 +2366,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10">
       <c r="A15" t="s">
         <v>22</v>
       </c>
@@ -2389,7 +2398,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10">
       <c r="A16" t="s">
         <v>23</v>
       </c>
@@ -2421,7 +2430,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10">
       <c r="A17" t="s">
         <v>24</v>
       </c>
@@ -2453,7 +2462,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10">
       <c r="A18" t="s">
         <v>25</v>
       </c>
@@ -2485,7 +2494,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10">
       <c r="A19" t="s">
         <v>26</v>
       </c>
@@ -2517,7 +2526,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10">
       <c r="A20" t="s">
         <v>27</v>
       </c>
@@ -2549,7 +2558,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10">
       <c r="A21" t="s">
         <v>28</v>
       </c>
@@ -2581,7 +2590,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10">
       <c r="A22" t="s">
         <v>29</v>
       </c>
@@ -2613,7 +2622,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10">
       <c r="A23" t="s">
         <v>30</v>
       </c>
@@ -2645,7 +2654,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10">
       <c r="A24" t="s">
         <v>31</v>
       </c>
@@ -2677,7 +2686,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10">
       <c r="A25" t="s">
         <v>32</v>
       </c>
@@ -2709,7 +2718,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10">
       <c r="A26" t="s">
         <v>33</v>
       </c>
@@ -2741,7 +2750,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10">
       <c r="A27" t="s">
         <v>34</v>
       </c>
@@ -2773,7 +2782,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10">
       <c r="A28" t="s">
         <v>35</v>
       </c>
@@ -2805,7 +2814,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10">
       <c r="A29" t="s">
         <v>36</v>
       </c>
@@ -2837,7 +2846,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10">
       <c r="A30" t="s">
         <v>37</v>
       </c>
@@ -2869,7 +2878,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10">
       <c r="A31" t="s">
         <v>38</v>
       </c>
@@ -2901,7 +2910,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10">
       <c r="A32" t="s">
         <v>39</v>
       </c>
@@ -2933,7 +2942,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10">
       <c r="A33" t="s">
         <v>40</v>
       </c>
@@ -2965,7 +2974,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10">
       <c r="A34" t="s">
         <v>41</v>
       </c>
@@ -2997,7 +3006,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10">
       <c r="A35" t="s">
         <v>42</v>
       </c>
@@ -3029,7 +3038,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10">
       <c r="A36" t="s">
         <v>43</v>
       </c>
@@ -3061,7 +3070,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10">
       <c r="A37" t="s">
         <v>44</v>
       </c>
@@ -3093,7 +3102,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10">
       <c r="A38" t="s">
         <v>45</v>
       </c>
@@ -3125,7 +3134,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10">
       <c r="A39" t="s">
         <v>46</v>
       </c>
@@ -3157,7 +3166,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10">
       <c r="A40" t="s">
         <v>47</v>
       </c>
@@ -3189,7 +3198,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10">
       <c r="A41" t="s">
         <v>48</v>
       </c>
@@ -3221,7 +3230,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10">
       <c r="A42" t="s">
         <v>49</v>
       </c>
@@ -3253,7 +3262,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10">
       <c r="A43" t="s">
         <v>50</v>
       </c>
@@ -3285,7 +3294,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10">
       <c r="A44" t="s">
         <v>51</v>
       </c>
@@ -3317,7 +3326,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10">
       <c r="A45" t="s">
         <v>52</v>
       </c>
@@ -3349,7 +3358,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10">
       <c r="A46" t="s">
         <v>53</v>
       </c>
@@ -3381,7 +3390,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10">
       <c r="A47" t="s">
         <v>54</v>
       </c>
@@ -3413,7 +3422,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10">
       <c r="A48" t="s">
         <v>55</v>
       </c>
@@ -3445,7 +3454,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10">
       <c r="A49" t="s">
         <v>56</v>
       </c>
@@ -3477,7 +3486,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10">
       <c r="A50" t="s">
         <v>57</v>
       </c>
@@ -3509,7 +3518,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10">
       <c r="A51" t="s">
         <v>58</v>
       </c>
@@ -3541,7 +3550,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10">
       <c r="A52" t="s">
         <v>59</v>
       </c>
@@ -3573,7 +3582,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10">
       <c r="A53" t="s">
         <v>60</v>
       </c>
@@ -3605,7 +3614,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10">
       <c r="A54" t="s">
         <v>61</v>
       </c>
@@ -3637,7 +3646,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10">
       <c r="A55" t="s">
         <v>62</v>
       </c>
@@ -3669,7 +3678,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:10">
       <c r="A56" t="s">
         <v>63</v>
       </c>
@@ -3701,7 +3710,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:10">
       <c r="A57" t="s">
         <v>64</v>
       </c>
@@ -3733,7 +3742,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10">
       <c r="A58" t="s">
         <v>65</v>
       </c>
@@ -3765,7 +3774,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:10">
       <c r="A59" t="s">
         <v>66</v>
       </c>
@@ -3797,7 +3806,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:10">
       <c r="A60" t="s">
         <v>67</v>
       </c>
@@ -3829,7 +3838,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:10">
       <c r="A61" t="s">
         <v>68</v>
       </c>
@@ -3861,7 +3870,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:10">
       <c r="A62" t="s">
         <v>69</v>
       </c>
@@ -3893,7 +3902,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:10">
       <c r="A63" t="s">
         <v>70</v>
       </c>
@@ -3925,7 +3934,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:10">
       <c r="A64" t="s">
         <v>71</v>
       </c>
@@ -3957,7 +3966,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:10">
       <c r="A65" t="s">
         <v>72</v>
       </c>
@@ -3989,7 +3998,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:10">
       <c r="A66" t="s">
         <v>73</v>
       </c>
@@ -4021,7 +4030,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:10">
       <c r="A67" t="s">
         <v>74</v>
       </c>
@@ -4053,7 +4062,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:10">
       <c r="A68" t="s">
         <v>75</v>
       </c>
@@ -4085,7 +4094,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:10">
       <c r="A69" t="s">
         <v>76</v>
       </c>
@@ -4117,7 +4126,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:10">
       <c r="A70" t="s">
         <v>77</v>
       </c>
@@ -4149,7 +4158,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:10">
       <c r="A71" t="s">
         <v>78</v>
       </c>
@@ -4181,7 +4190,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:10">
       <c r="A72" t="s">
         <v>79</v>
       </c>
@@ -4213,7 +4222,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:10">
       <c r="A73" t="s">
         <v>80</v>
       </c>
@@ -4245,7 +4254,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:10">
       <c r="A74" t="s">
         <v>81</v>
       </c>
@@ -4277,7 +4286,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:10">
       <c r="A75" t="s">
         <v>82</v>
       </c>
@@ -4309,7 +4318,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:10">
       <c r="A76" t="s">
         <v>83</v>
       </c>
@@ -4341,7 +4350,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:10">
       <c r="A77" t="s">
         <v>84</v>
       </c>
@@ -4373,7 +4382,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:10">
       <c r="A78" t="s">
         <v>85</v>
       </c>
@@ -4405,7 +4414,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:10">
       <c r="A79" t="s">
         <v>86</v>
       </c>
@@ -4437,7 +4446,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:10">
       <c r="A80" t="s">
         <v>87</v>
       </c>
@@ -4469,7 +4478,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:10">
       <c r="A81" t="s">
         <v>88</v>
       </c>
@@ -4501,7 +4510,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:10">
       <c r="A82" t="s">
         <v>89</v>
       </c>
@@ -4533,7 +4542,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:10">
       <c r="A83" t="s">
         <v>90</v>
       </c>
@@ -4565,7 +4574,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:10">
       <c r="A84" t="s">
         <v>91</v>
       </c>
@@ -4597,7 +4606,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:10">
       <c r="A85" t="s">
         <v>92</v>
       </c>
@@ -4629,7 +4638,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:10">
       <c r="A86" t="s">
         <v>93</v>
       </c>
@@ -4661,7 +4670,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:10">
       <c r="A87" t="s">
         <v>94</v>
       </c>
@@ -4693,7 +4702,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:10">
       <c r="A88" t="s">
         <v>95</v>
       </c>
@@ -4725,7 +4734,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:10">
       <c r="A89" t="s">
         <v>96</v>
       </c>
@@ -4757,7 +4766,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:10">
       <c r="A90" t="s">
         <v>97</v>
       </c>
@@ -4789,7 +4798,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:10">
       <c r="A91" t="s">
         <v>98</v>
       </c>
@@ -4821,7 +4830,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:10">
       <c r="A92" t="s">
         <v>99</v>
       </c>
@@ -4853,7 +4862,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:10">
       <c r="A93" t="s">
         <v>100</v>
       </c>
@@ -4885,7 +4894,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:10">
       <c r="A94" t="s">
         <v>101</v>
       </c>
@@ -4917,7 +4926,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:10">
       <c r="A95" t="s">
         <v>102</v>
       </c>
@@ -4949,7 +4958,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:10">
       <c r="A96" t="s">
         <v>103</v>
       </c>
@@ -4981,7 +4990,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:10">
       <c r="A97" t="s">
         <v>104</v>
       </c>
@@ -5013,7 +5022,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:10">
       <c r="A98" t="s">
         <v>105</v>
       </c>
@@ -5045,7 +5054,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:10">
       <c r="A99" t="s">
         <v>106</v>
       </c>
@@ -5077,7 +5086,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:10">
       <c r="A100" t="s">
         <v>107</v>
       </c>
@@ -5109,7 +5118,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:10">
       <c r="A101" t="s">
         <v>108</v>
       </c>
@@ -5141,7 +5150,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:10">
       <c r="A102" t="s">
         <v>109</v>
       </c>
@@ -5173,7 +5182,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:10">
       <c r="A103" t="s">
         <v>110</v>
       </c>
@@ -5205,7 +5214,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:10">
       <c r="A104" t="s">
         <v>111</v>
       </c>
@@ -5237,7 +5246,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:10">
       <c r="A105" t="s">
         <v>112</v>
       </c>
@@ -5269,7 +5278,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:10">
       <c r="A106" t="s">
         <v>113</v>
       </c>
@@ -5301,7 +5310,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:10">
       <c r="A107" t="s">
         <v>114</v>
       </c>
@@ -5333,7 +5342,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:10">
       <c r="A108" t="s">
         <v>115</v>
       </c>
@@ -5365,7 +5374,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:10">
       <c r="A109" t="s">
         <v>116</v>
       </c>
@@ -5397,7 +5406,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:10">
       <c r="A110" t="s">
         <v>117</v>
       </c>
@@ -5429,7 +5438,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:10">
       <c r="A111" t="s">
         <v>118</v>
       </c>
@@ -5461,7 +5470,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:10">
       <c r="A112" t="s">
         <v>119</v>
       </c>
@@ -5493,7 +5502,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:10">
       <c r="A113" t="s">
         <v>120</v>
       </c>
@@ -5525,7 +5534,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="114" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:10">
       <c r="A114" t="s">
         <v>121</v>
       </c>
@@ -5557,7 +5566,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:10">
       <c r="A115" t="s">
         <v>122</v>
       </c>
@@ -5589,7 +5598,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="116" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:10">
       <c r="A116" t="s">
         <v>123</v>
       </c>
@@ -5621,7 +5630,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:10">
       <c r="A117" t="s">
         <v>124</v>
       </c>
@@ -5653,7 +5662,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="118" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:10">
       <c r="A118" t="s">
         <v>125</v>
       </c>
@@ -5685,7 +5694,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:10">
       <c r="A119" t="s">
         <v>126</v>
       </c>
@@ -5717,7 +5726,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="120" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:10">
       <c r="A120" t="s">
         <v>127</v>
       </c>
@@ -5749,7 +5758,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:10">
       <c r="A121" t="s">
         <v>128</v>
       </c>
@@ -5781,7 +5790,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="122" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:10">
       <c r="A122" t="s">
         <v>129</v>
       </c>
@@ -5813,7 +5822,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:10">
       <c r="A123" t="s">
         <v>130</v>
       </c>
@@ -5845,7 +5854,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="124" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:10">
       <c r="A124" t="s">
         <v>131</v>
       </c>
@@ -5877,7 +5886,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:10">
       <c r="A125" t="s">
         <v>132</v>
       </c>
@@ -5909,7 +5918,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="126" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:10">
       <c r="A126" t="s">
         <v>133</v>
       </c>
@@ -5941,7 +5950,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:10">
       <c r="A127" t="s">
         <v>134</v>
       </c>
@@ -5973,7 +5982,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="128" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:10">
       <c r="A128" t="s">
         <v>135</v>
       </c>
@@ -6005,7 +6014,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="129" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:10">
       <c r="A129" t="s">
         <v>136</v>
       </c>
@@ -6037,7 +6046,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="130" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:10">
       <c r="A130" t="s">
         <v>137</v>
       </c>
@@ -6069,7 +6078,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:10">
       <c r="A131" t="s">
         <v>138</v>
       </c>
@@ -6101,7 +6110,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="132" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:10">
       <c r="A132" t="s">
         <v>139</v>
       </c>
@@ -6133,7 +6142,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:10">
       <c r="A133" t="s">
         <v>140</v>
       </c>
@@ -6165,7 +6174,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="134" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:10">
       <c r="A134" t="s">
         <v>141</v>
       </c>
@@ -6197,7 +6206,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="135" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:10">
       <c r="A135" t="s">
         <v>142</v>
       </c>
@@ -6229,7 +6238,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="136" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:10">
       <c r="A136" t="s">
         <v>143</v>
       </c>
@@ -6261,7 +6270,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="137" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:10">
       <c r="A137" t="s">
         <v>144</v>
       </c>
@@ -6293,7 +6302,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="138" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:10">
       <c r="A138" t="s">
         <v>145</v>
       </c>
@@ -6325,7 +6334,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="139" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:10">
       <c r="A139" t="s">
         <v>146</v>
       </c>
@@ -6357,7 +6366,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="140" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:10">
       <c r="A140" t="s">
         <v>147</v>
       </c>
@@ -6389,7 +6398,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="141" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:10">
       <c r="A141" t="s">
         <v>148</v>
       </c>
@@ -6421,7 +6430,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="142" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:10">
       <c r="A142" t="s">
         <v>149</v>
       </c>
@@ -6453,7 +6462,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="143" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:10">
       <c r="A143" t="s">
         <v>150</v>
       </c>
@@ -6485,7 +6494,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="144" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:10">
       <c r="A144" t="s">
         <v>151</v>
       </c>
@@ -6517,7 +6526,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="145" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:10">
       <c r="A145" t="s">
         <v>152</v>
       </c>
@@ -6549,7 +6558,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="146" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:10">
       <c r="A146" t="s">
         <v>153</v>
       </c>
@@ -6581,7 +6590,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="147" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:10">
       <c r="A147" t="s">
         <v>154</v>
       </c>
@@ -6613,7 +6622,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="148" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:10">
       <c r="A148" t="s">
         <v>155</v>
       </c>
@@ -6645,7 +6654,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="149" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:10">
       <c r="A149" t="s">
         <v>156</v>
       </c>
@@ -6677,7 +6686,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="150" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:10">
       <c r="A150" t="s">
         <v>157</v>
       </c>
@@ -6709,7 +6718,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="151" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:10">
       <c r="A151" t="s">
         <v>158</v>
       </c>
@@ -6741,7 +6750,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="152" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:10">
       <c r="A152" t="s">
         <v>159</v>
       </c>
@@ -6773,7 +6782,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="153" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:10">
       <c r="A153" t="s">
         <v>160</v>
       </c>
@@ -6805,7 +6814,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="154" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:10">
       <c r="A154" t="s">
         <v>161</v>
       </c>
@@ -6837,7 +6846,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="155" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:10">
       <c r="A155" t="s">
         <v>162</v>
       </c>
@@ -6869,7 +6878,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="156" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:10">
       <c r="A156" t="s">
         <v>163</v>
       </c>
@@ -6901,7 +6910,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="157" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:10">
       <c r="A157" t="s">
         <v>164</v>
       </c>
@@ -6933,7 +6942,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="158" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:10">
       <c r="A158" t="s">
         <v>165</v>
       </c>
@@ -6965,7 +6974,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="159" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:10">
       <c r="A159" t="s">
         <v>166</v>
       </c>
@@ -6997,7 +7006,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="160" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:10">
       <c r="A160" t="s">
         <v>167</v>
       </c>
@@ -7029,7 +7038,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="161" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:10">
       <c r="A161" t="s">
         <v>168</v>
       </c>
@@ -7061,7 +7070,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="162" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:10">
       <c r="A162" t="s">
         <v>169</v>
       </c>
@@ -7093,7 +7102,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="163" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:10">
       <c r="A163" t="s">
         <v>170</v>
       </c>
@@ -7125,7 +7134,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="164" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:10">
       <c r="A164" t="s">
         <v>171</v>
       </c>
@@ -7157,7 +7166,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="165" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:10">
       <c r="A165" t="s">
         <v>172</v>
       </c>
@@ -7189,7 +7198,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="166" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:10">
       <c r="A166" t="s">
         <v>173</v>
       </c>
@@ -7221,7 +7230,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="167" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:10">
       <c r="A167" t="s">
         <v>174</v>
       </c>
@@ -7253,7 +7262,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="168" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:10">
       <c r="A168" t="s">
         <v>175</v>
       </c>
@@ -7285,7 +7294,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="169" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:10">
       <c r="A169" t="s">
         <v>176</v>
       </c>
@@ -7317,7 +7326,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="170" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:10">
       <c r="A170" t="s">
         <v>177</v>
       </c>
@@ -7349,7 +7358,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="171" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:10">
       <c r="A171" t="s">
         <v>178</v>
       </c>
@@ -7381,7 +7390,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="172" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:10">
       <c r="A172" t="s">
         <v>179</v>
       </c>
@@ -7413,7 +7422,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="173" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:10">
       <c r="A173" t="s">
         <v>180</v>
       </c>
@@ -7445,7 +7454,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="174" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:10">
       <c r="A174" t="s">
         <v>181</v>
       </c>
@@ -7477,7 +7486,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="175" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:10">
       <c r="A175" t="s">
         <v>182</v>
       </c>
@@ -7509,7 +7518,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="176" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:10">
       <c r="A176" t="s">
         <v>183</v>
       </c>
@@ -7541,7 +7550,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="177" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:10">
       <c r="A177" t="s">
         <v>184</v>
       </c>
@@ -7573,7 +7582,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="178" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:10">
       <c r="A178" t="s">
         <v>185</v>
       </c>
@@ -7605,7 +7614,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="179" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:10">
       <c r="A179" t="s">
         <v>186</v>
       </c>
@@ -7637,7 +7646,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="180" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:10">
       <c r="A180" t="s">
         <v>187</v>
       </c>
@@ -7669,7 +7678,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="181" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:10">
       <c r="A181" t="s">
         <v>188</v>
       </c>
@@ -7701,7 +7710,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="182" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:10">
       <c r="A182" t="s">
         <v>189</v>
       </c>
@@ -7733,7 +7742,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="183" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:10">
       <c r="A183" t="s">
         <v>190</v>
       </c>
@@ -7765,7 +7774,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="184" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:10">
       <c r="A184" t="s">
         <v>191</v>
       </c>
@@ -7797,7 +7806,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="185" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:10">
       <c r="A185" t="s">
         <v>192</v>
       </c>
@@ -7829,7 +7838,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="186" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:10">
       <c r="A186" t="s">
         <v>193</v>
       </c>
@@ -7861,7 +7870,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="187" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:10">
       <c r="A187" t="s">
         <v>194</v>
       </c>
@@ -7893,7 +7902,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="188" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:10">
       <c r="A188" t="s">
         <v>195</v>
       </c>
@@ -7925,7 +7934,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="189" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:10">
       <c r="A189" t="s">
         <v>196</v>
       </c>
@@ -7957,7 +7966,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="190" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:10">
       <c r="A190" t="s">
         <v>197</v>
       </c>
@@ -7989,7 +7998,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="191" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:10">
       <c r="A191" t="s">
         <v>198</v>
       </c>
@@ -8021,7 +8030,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="192" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:10">
       <c r="A192" t="s">
         <v>199</v>
       </c>
@@ -8053,7 +8062,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="193" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:10">
       <c r="A193" t="s">
         <v>200</v>
       </c>
@@ -8085,7 +8094,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="194" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:10">
       <c r="A194" t="s">
         <v>201</v>
       </c>
@@ -8117,7 +8126,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="195" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:10">
       <c r="A195" t="s">
         <v>202</v>
       </c>
@@ -8149,7 +8158,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="196" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:10">
       <c r="A196" t="s">
         <v>203</v>
       </c>
@@ -8181,7 +8190,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="197" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:10">
       <c r="A197" t="s">
         <v>204</v>
       </c>
@@ -8213,7 +8222,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="198" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:10">
       <c r="A198" t="s">
         <v>205</v>
       </c>
@@ -8245,7 +8254,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="199" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:10">
       <c r="A199" t="s">
         <v>206</v>
       </c>
@@ -8277,7 +8286,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="200" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:10">
       <c r="A200" t="s">
         <v>207</v>
       </c>
@@ -8309,7 +8318,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="201" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:10">
       <c r="A201" t="s">
         <v>208</v>
       </c>
@@ -8341,7 +8350,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="202" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:10">
       <c r="A202" t="s">
         <v>209</v>
       </c>
@@ -8373,7 +8382,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="203" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:10">
       <c r="A203" t="s">
         <v>210</v>
       </c>
@@ -8405,7 +8414,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="204" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:10">
       <c r="A204" t="s">
         <v>211</v>
       </c>
@@ -8437,7 +8446,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="205" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:10">
       <c r="A205" t="s">
         <v>212</v>
       </c>
@@ -8469,7 +8478,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="206" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:10">
       <c r="A206" t="s">
         <v>213</v>
       </c>
@@ -8501,7 +8510,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="207" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:10">
       <c r="A207" t="s">
         <v>214</v>
       </c>
@@ -8533,7 +8542,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="208" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:10">
       <c r="A208" t="s">
         <v>215</v>
       </c>
@@ -8565,7 +8574,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="209" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:10">
       <c r="A209" t="s">
         <v>216</v>
       </c>
@@ -8597,7 +8606,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="210" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:10">
       <c r="A210" t="s">
         <v>217</v>
       </c>
@@ -8629,7 +8638,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="211" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:10">
       <c r="A211" t="s">
         <v>218</v>
       </c>
@@ -8661,7 +8670,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="212" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:10">
       <c r="A212" t="s">
         <v>219</v>
       </c>
@@ -8693,7 +8702,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="213" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:10">
       <c r="A213" t="s">
         <v>220</v>
       </c>
@@ -8725,7 +8734,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="214" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:10">
       <c r="A214" t="s">
         <v>221</v>
       </c>
@@ -8757,7 +8766,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="215" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:10">
       <c r="A215" t="s">
         <v>222</v>
       </c>
@@ -8789,7 +8798,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="216" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:10">
       <c r="A216" t="s">
         <v>223</v>
       </c>
@@ -8821,7 +8830,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="217" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:10">
       <c r="A217" t="s">
         <v>224</v>
       </c>
@@ -8853,7 +8862,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="218" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:10">
       <c r="A218" t="s">
         <v>225</v>
       </c>
@@ -8885,7 +8894,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="219" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:10">
       <c r="A219" t="s">
         <v>226</v>
       </c>
@@ -8917,7 +8926,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="220" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:10">
       <c r="A220" t="s">
         <v>227</v>
       </c>
@@ -8949,7 +8958,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="221" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:10">
       <c r="A221" t="s">
         <v>228</v>
       </c>
@@ -8981,7 +8990,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="222" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:10">
       <c r="A222" t="s">
         <v>229</v>
       </c>
@@ -9013,7 +9022,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="223" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:10">
       <c r="A223" t="s">
         <v>230</v>
       </c>
@@ -9045,7 +9054,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="224" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:10">
       <c r="A224" t="s">
         <v>231</v>
       </c>
@@ -9077,7 +9086,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="225" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:10">
       <c r="A225" t="s">
         <v>232</v>
       </c>
@@ -9109,7 +9118,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="226" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:10">
       <c r="A226" t="s">
         <v>233</v>
       </c>
@@ -9141,7 +9150,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="227" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:10">
       <c r="A227" t="s">
         <v>234</v>
       </c>
@@ -9173,7 +9182,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="228" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:10">
       <c r="A228" t="s">
         <v>235</v>
       </c>
@@ -9205,7 +9214,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="229" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:10">
       <c r="A229" t="s">
         <v>236</v>
       </c>
@@ -9237,7 +9246,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="230" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:10">
       <c r="A230" t="s">
         <v>237</v>
       </c>
@@ -9269,7 +9278,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="231" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:10">
       <c r="A231" t="s">
         <v>238</v>
       </c>
@@ -9301,7 +9310,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="232" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:10">
       <c r="A232" t="s">
         <v>239</v>
       </c>
@@ -9333,7 +9342,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="233" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:10">
       <c r="A233" t="s">
         <v>240</v>
       </c>
@@ -9365,7 +9374,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="234" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:10">
       <c r="A234" t="s">
         <v>241</v>
       </c>
@@ -9397,7 +9406,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="235" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:10">
       <c r="A235" t="s">
         <v>242</v>
       </c>
@@ -9429,7 +9438,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="236" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:10">
       <c r="A236" t="s">
         <v>243</v>
       </c>
@@ -9461,7 +9470,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="237" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:10">
       <c r="A237" t="s">
         <v>244</v>
       </c>
@@ -9493,7 +9502,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="238" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:10">
       <c r="A238" t="s">
         <v>245</v>
       </c>
@@ -9525,7 +9534,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="239" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:10">
       <c r="A239" t="s">
         <v>246</v>
       </c>
@@ -9557,7 +9566,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="240" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:10">
       <c r="A240" t="s">
         <v>247</v>
       </c>
@@ -9589,7 +9598,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="241" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:10">
       <c r="A241" t="s">
         <v>248</v>
       </c>
@@ -9621,7 +9630,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="242" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:10">
       <c r="A242" t="s">
         <v>249</v>
       </c>
@@ -9653,7 +9662,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="243" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:10">
       <c r="A243" t="s">
         <v>250</v>
       </c>
@@ -9685,7 +9694,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="244" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:10">
       <c r="A244" t="s">
         <v>251</v>
       </c>
@@ -9717,7 +9726,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="245" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:10">
       <c r="A245" t="s">
         <v>252</v>
       </c>
@@ -9749,7 +9758,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="246" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:10">
       <c r="A246" t="s">
         <v>253</v>
       </c>
@@ -9781,7 +9790,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="247" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:10">
       <c r="A247" t="s">
         <v>254</v>
       </c>
@@ -9813,7 +9822,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="248" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:10">
       <c r="A248" t="s">
         <v>255</v>
       </c>
@@ -9845,7 +9854,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="249" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:10">
       <c r="A249" t="s">
         <v>256</v>
       </c>
@@ -9877,7 +9886,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="250" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:10">
       <c r="A250" t="s">
         <v>257</v>
       </c>
@@ -9909,7 +9918,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="251" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:10">
       <c r="A251" t="s">
         <v>258</v>
       </c>
@@ -9941,7 +9950,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="252" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:10">
       <c r="A252" t="s">
         <v>259</v>
       </c>
@@ -9973,7 +9982,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="253" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:10">
       <c r="A253" t="s">
         <v>260</v>
       </c>
@@ -10005,7 +10014,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="254" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:10">
       <c r="A254" t="s">
         <v>261</v>
       </c>
@@ -10037,7 +10046,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="255" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:10">
       <c r="A255" t="s">
         <v>262</v>
       </c>
@@ -10069,7 +10078,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="256" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:10">
       <c r="A256" t="s">
         <v>263</v>
       </c>
@@ -10101,7 +10110,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="257" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:10">
       <c r="A257" t="s">
         <v>264</v>
       </c>
@@ -10133,7 +10142,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="258" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:10">
       <c r="A258" t="s">
         <v>265</v>
       </c>
@@ -10165,7 +10174,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="259" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:10">
       <c r="A259" t="s">
         <v>266</v>
       </c>
@@ -10197,7 +10206,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="260" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:10">
       <c r="A260" t="s">
         <v>267</v>
       </c>
@@ -10229,7 +10238,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="261" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:10">
       <c r="A261" t="s">
         <v>268</v>
       </c>
@@ -10261,7 +10270,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="262" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:10">
       <c r="A262" t="s">
         <v>269</v>
       </c>
@@ -10293,7 +10302,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="263" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:10">
       <c r="A263" t="s">
         <v>270</v>
       </c>
@@ -10325,7 +10334,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="264" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:10">
       <c r="A264" t="s">
         <v>271</v>
       </c>
@@ -10357,7 +10366,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="265" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:10">
       <c r="A265" t="s">
         <v>272</v>
       </c>
@@ -10389,7 +10398,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="266" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:10">
       <c r="A266" t="s">
         <v>273</v>
       </c>
@@ -10421,7 +10430,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="267" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:10">
       <c r="A267" t="s">
         <v>274</v>
       </c>
@@ -10453,7 +10462,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="268" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:10">
       <c r="A268" t="s">
         <v>275</v>
       </c>
@@ -10485,7 +10494,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="269" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:10">
       <c r="A269" t="s">
         <v>276</v>
       </c>
@@ -10517,7 +10526,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="270" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:10">
       <c r="A270" t="s">
         <v>277</v>
       </c>
@@ -10549,7 +10558,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="271" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:10">
       <c r="A271" t="s">
         <v>278</v>
       </c>
@@ -10581,7 +10590,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="272" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:10">
       <c r="A272" t="s">
         <v>279</v>
       </c>
@@ -10613,7 +10622,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="273" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:10">
       <c r="A273" t="s">
         <v>280</v>
       </c>
@@ -10645,7 +10654,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="274" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:10">
       <c r="A274" t="s">
         <v>281</v>
       </c>
@@ -10677,7 +10686,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="275" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:10">
       <c r="A275" t="s">
         <v>282</v>
       </c>
@@ -10709,7 +10718,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="276" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:10">
       <c r="A276" t="s">
         <v>283</v>
       </c>
@@ -10741,7 +10750,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="277" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:10">
       <c r="A277" t="s">
         <v>284</v>
       </c>
@@ -10773,7 +10782,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="278" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:10">
       <c r="A278" t="s">
         <v>285</v>
       </c>
@@ -10805,7 +10814,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="279" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:10">
       <c r="A279" t="s">
         <v>286</v>
       </c>
@@ -10837,7 +10846,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="280" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:10">
       <c r="A280" t="s">
         <v>287</v>
       </c>
@@ -10869,7 +10878,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="281" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:10">
       <c r="A281" t="s">
         <v>288</v>
       </c>
@@ -10901,7 +10910,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="282" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:10">
       <c r="A282" t="s">
         <v>289</v>
       </c>
@@ -10933,7 +10942,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="283" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:10">
       <c r="A283" t="s">
         <v>290</v>
       </c>
@@ -10965,7 +10974,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="284" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:10">
       <c r="A284" t="s">
         <v>291</v>
       </c>
@@ -10997,7 +11006,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="285" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:10">
       <c r="A285" t="s">
         <v>292</v>
       </c>
@@ -11029,7 +11038,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="286" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:10">
       <c r="A286" t="s">
         <v>293</v>
       </c>
@@ -11061,7 +11070,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="287" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:10">
       <c r="A287" t="s">
         <v>294</v>
       </c>
@@ -11093,7 +11102,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="288" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:10">
       <c r="A288" t="s">
         <v>295</v>
       </c>
@@ -11125,7 +11134,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="289" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:10">
       <c r="A289" t="s">
         <v>296</v>
       </c>
@@ -11157,7 +11166,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="290" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:10">
       <c r="A290" t="s">
         <v>297</v>
       </c>
@@ -11189,7 +11198,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="291" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:10">
       <c r="A291" t="s">
         <v>298</v>
       </c>
@@ -11221,7 +11230,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="292" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:10">
       <c r="A292" t="s">
         <v>299</v>
       </c>
@@ -11253,7 +11262,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="293" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:10">
       <c r="A293" t="s">
         <v>300</v>
       </c>
@@ -11285,7 +11294,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="294" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:10">
       <c r="A294" t="s">
         <v>301</v>
       </c>
@@ -11317,7 +11326,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="295" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:10">
       <c r="A295" t="s">
         <v>302</v>
       </c>
@@ -11349,7 +11358,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="296" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:10">
       <c r="A296" t="s">
         <v>303</v>
       </c>
@@ -11381,7 +11390,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="297" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:10">
       <c r="A297" t="s">
         <v>304</v>
       </c>
@@ -11413,7 +11422,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="298" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:10">
       <c r="A298" t="s">
         <v>305</v>
       </c>
@@ -11445,7 +11454,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="299" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:10">
       <c r="A299" t="s">
         <v>306</v>
       </c>
@@ -11477,7 +11486,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="300" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:10">
       <c r="A300" t="s">
         <v>307</v>
       </c>
@@ -11509,7 +11518,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="301" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:10">
       <c r="A301" t="s">
         <v>308</v>
       </c>
@@ -11541,7 +11550,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="302" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:10">
       <c r="A302" t="s">
         <v>309</v>
       </c>
@@ -11573,7 +11582,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="303" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:10">
       <c r="A303" t="s">
         <v>310</v>
       </c>
@@ -11605,7 +11614,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="304" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:10">
       <c r="A304" t="s">
         <v>311</v>
       </c>
@@ -11637,7 +11646,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="305" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:10">
       <c r="A305" t="s">
         <v>312</v>
       </c>
@@ -11669,7 +11678,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="306" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:10">
       <c r="A306" t="s">
         <v>313</v>
       </c>
@@ -11701,7 +11710,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="307" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:10">
       <c r="A307" t="s">
         <v>314</v>
       </c>
@@ -11733,7 +11742,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="308" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:10">
       <c r="A308" t="s">
         <v>315</v>
       </c>
@@ -11765,7 +11774,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="309" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:10">
       <c r="A309" t="s">
         <v>316</v>
       </c>
@@ -11797,7 +11806,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="310" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:10">
       <c r="A310" t="s">
         <v>317</v>
       </c>
@@ -11829,7 +11838,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="311" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:10">
       <c r="A311" t="s">
         <v>318</v>
       </c>
@@ -11861,7 +11870,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="312" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:10">
       <c r="A312" t="s">
         <v>319</v>
       </c>
@@ -11893,7 +11902,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="313" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:10">
       <c r="A313" t="s">
         <v>320</v>
       </c>
@@ -11925,7 +11934,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="314" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:10">
       <c r="A314" t="s">
         <v>321</v>
       </c>
@@ -11957,7 +11966,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="315" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:10">
       <c r="A315" t="s">
         <v>322</v>
       </c>
@@ -11989,7 +11998,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="316" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:10">
       <c r="A316" t="s">
         <v>323</v>
       </c>
@@ -12021,7 +12030,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="317" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:10">
       <c r="A317" t="s">
         <v>324</v>
       </c>
@@ -12053,7 +12062,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="318" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:10">
       <c r="A318" t="s">
         <v>325</v>
       </c>
@@ -12085,7 +12094,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="319" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:10">
       <c r="A319" t="s">
         <v>326</v>
       </c>
@@ -12117,7 +12126,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="320" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:10">
       <c r="A320" t="s">
         <v>327</v>
       </c>
@@ -12149,7 +12158,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="321" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:10">
       <c r="A321" t="s">
         <v>328</v>
       </c>
@@ -12181,7 +12190,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="322" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:10">
       <c r="A322" t="s">
         <v>329</v>
       </c>
@@ -12213,7 +12222,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="323" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:10">
       <c r="A323" t="s">
         <v>330</v>
       </c>
@@ -12245,7 +12254,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="324" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:10">
       <c r="A324" t="s">
         <v>331</v>
       </c>
@@ -12277,7 +12286,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="325" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:10">
       <c r="A325" t="s">
         <v>332</v>
       </c>
@@ -12309,7 +12318,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="326" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:10">
       <c r="A326" t="s">
         <v>333</v>
       </c>
@@ -12341,7 +12350,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="327" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:10">
       <c r="A327" t="s">
         <v>334</v>
       </c>
@@ -12373,7 +12382,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="328" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:10">
       <c r="A328" t="s">
         <v>335</v>
       </c>
@@ -12405,7 +12414,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="329" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:10">
       <c r="A329" t="s">
         <v>336</v>
       </c>
@@ -12437,7 +12446,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="330" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:10">
       <c r="A330" t="s">
         <v>337</v>
       </c>
@@ -12469,7 +12478,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="331" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:10">
       <c r="A331" t="s">
         <v>338</v>
       </c>
@@ -12501,7 +12510,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="332" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:10">
       <c r="A332" t="s">
         <v>339</v>
       </c>
@@ -12533,7 +12542,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="333" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:10">
       <c r="A333" t="s">
         <v>340</v>
       </c>
@@ -12565,7 +12574,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="334" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:10">
       <c r="A334" t="s">
         <v>341</v>
       </c>
@@ -12597,7 +12606,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="335" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:10">
       <c r="A335" t="s">
         <v>342</v>
       </c>
@@ -12629,7 +12638,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="336" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:10">
       <c r="A336" t="s">
         <v>343</v>
       </c>
@@ -12661,7 +12670,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="337" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:10">
       <c r="A337" t="s">
         <v>344</v>
       </c>
@@ -12693,7 +12702,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="338" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:10">
       <c r="A338" t="s">
         <v>345</v>
       </c>
@@ -12725,7 +12734,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="339" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:10">
       <c r="A339" t="s">
         <v>346</v>
       </c>
@@ -12757,7 +12766,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="340" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:10">
       <c r="A340" t="s">
         <v>347</v>
       </c>
@@ -12789,7 +12798,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="341" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:10">
       <c r="A341" t="s">
         <v>348</v>
       </c>
@@ -12821,7 +12830,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="342" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:10">
       <c r="A342" t="s">
         <v>349</v>
       </c>
@@ -12853,7 +12862,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="343" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:10">
       <c r="A343" t="s">
         <v>350</v>
       </c>
@@ -12885,7 +12894,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="344" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:10">
       <c r="A344" t="s">
         <v>351</v>
       </c>
@@ -12917,7 +12926,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="345" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:10">
       <c r="A345" t="s">
         <v>352</v>
       </c>
@@ -12949,7 +12958,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="346" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:10">
       <c r="A346" t="s">
         <v>353</v>
       </c>
@@ -12981,7 +12990,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="347" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:10">
       <c r="A347" t="s">
         <v>354</v>
       </c>
@@ -13013,7 +13022,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="348" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:10">
       <c r="A348" t="s">
         <v>355</v>
       </c>
@@ -13045,7 +13054,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="349" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:10">
       <c r="A349" t="s">
         <v>356</v>
       </c>
@@ -13077,7 +13086,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="350" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:10">
       <c r="A350" t="s">
         <v>357</v>
       </c>
@@ -13109,7 +13118,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="351" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:10">
       <c r="A351" t="s">
         <v>358</v>
       </c>
@@ -13141,7 +13150,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="352" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:10">
       <c r="A352" t="s">
         <v>359</v>
       </c>
@@ -13173,7 +13182,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="353" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:10">
       <c r="A353" t="s">
         <v>360</v>
       </c>
@@ -13205,7 +13214,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="354" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:10">
       <c r="A354" t="s">
         <v>361</v>
       </c>
@@ -13237,7 +13246,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="355" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:10">
       <c r="A355" t="s">
         <v>362</v>
       </c>
@@ -13269,7 +13278,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="356" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:10">
       <c r="A356" t="s">
         <v>363</v>
       </c>
@@ -13301,7 +13310,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="357" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:10">
       <c r="A357" t="s">
         <v>364</v>
       </c>
@@ -13333,7 +13342,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="358" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:10">
       <c r="A358" t="s">
         <v>365</v>
       </c>
@@ -13365,7 +13374,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="359" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:10">
       <c r="A359" t="s">
         <v>366</v>
       </c>
@@ -13397,7 +13406,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="360" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:10">
       <c r="A360" t="s">
         <v>367</v>
       </c>
@@ -13429,7 +13438,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="361" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:10">
       <c r="A361" t="s">
         <v>368</v>
       </c>
@@ -13461,7 +13470,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="362" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:10">
       <c r="A362" t="s">
         <v>369</v>
       </c>
@@ -13493,7 +13502,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="363" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:10">
       <c r="A363" t="s">
         <v>370</v>
       </c>
@@ -13525,7 +13534,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="364" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:10">
       <c r="A364" t="s">
         <v>371</v>
       </c>
@@ -13557,7 +13566,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="365" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:10">
       <c r="A365" t="s">
         <v>372</v>
       </c>
@@ -13589,7 +13598,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="366" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:10">
       <c r="A366" t="s">
         <v>373</v>
       </c>
@@ -13621,7 +13630,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="367" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:10">
       <c r="A367" t="s">
         <v>374</v>
       </c>
@@ -13653,7 +13662,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="368" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:10">
       <c r="A368" t="s">
         <v>375</v>
       </c>
@@ -13685,7 +13694,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="369" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="369" spans="1:10">
       <c r="A369" t="s">
         <v>376</v>
       </c>
@@ -13717,7 +13726,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="370" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="370" spans="1:10">
       <c r="A370" t="s">
         <v>377</v>
       </c>
@@ -13749,7 +13758,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="371" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="371" spans="1:10">
       <c r="A371" t="s">
         <v>378</v>
       </c>
@@ -13781,7 +13790,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="372" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="372" spans="1:10">
       <c r="A372" t="s">
         <v>379</v>
       </c>
@@ -13813,7 +13822,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="373" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="373" spans="1:10">
       <c r="A373" t="s">
         <v>380</v>
       </c>
@@ -13845,7 +13854,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="374" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="374" spans="1:10">
       <c r="A374" t="s">
         <v>381</v>
       </c>
@@ -13877,7 +13886,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="375" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="375" spans="1:10">
       <c r="A375" t="s">
         <v>382</v>
       </c>
@@ -13909,7 +13918,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="376" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="376" spans="1:10">
       <c r="A376" t="s">
         <v>383</v>
       </c>
@@ -13941,7 +13950,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="377" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="377" spans="1:10">
       <c r="A377" t="s">
         <v>384</v>
       </c>
@@ -13973,7 +13982,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="378" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="378" spans="1:10">
       <c r="A378" t="s">
         <v>385</v>
       </c>
@@ -14005,7 +14014,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="379" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="379" spans="1:10">
       <c r="A379" t="s">
         <v>386</v>
       </c>
@@ -14037,7 +14046,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="380" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="380" spans="1:10">
       <c r="A380" t="s">
         <v>387</v>
       </c>
@@ -14069,7 +14078,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="381" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="381" spans="1:10">
       <c r="A381" t="s">
         <v>388</v>
       </c>
@@ -14101,7 +14110,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="382" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="382" spans="1:10">
       <c r="A382" t="s">
         <v>389</v>
       </c>
@@ -14133,7 +14142,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="383" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="383" spans="1:10">
       <c r="A383" t="s">
         <v>390</v>
       </c>
@@ -14165,7 +14174,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="384" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="384" spans="1:10">
       <c r="A384" t="s">
         <v>391</v>
       </c>
@@ -14197,7 +14206,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="385" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="385" spans="1:10">
       <c r="A385" t="s">
         <v>392</v>
       </c>
@@ -14229,7 +14238,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="386" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="386" spans="1:10">
       <c r="A386" t="s">
         <v>393</v>
       </c>
@@ -14261,7 +14270,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="387" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="387" spans="1:10">
       <c r="A387" t="s">
         <v>394</v>
       </c>
@@ -14293,7 +14302,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="388" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="388" spans="1:10">
       <c r="A388" t="s">
         <v>395</v>
       </c>
@@ -14325,7 +14334,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="389" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="389" spans="1:10">
       <c r="A389" t="s">
         <v>396</v>
       </c>
@@ -14357,7 +14366,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="390" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="390" spans="1:10">
       <c r="A390" t="s">
         <v>397</v>
       </c>
@@ -14389,7 +14398,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="391" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="391" spans="1:10">
       <c r="A391" t="s">
         <v>398</v>
       </c>
@@ -14421,7 +14430,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="392" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="392" spans="1:10">
       <c r="A392" t="s">
         <v>399</v>
       </c>
@@ -14453,7 +14462,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="393" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="393" spans="1:10">
       <c r="A393" t="s">
         <v>400</v>
       </c>
@@ -14485,7 +14494,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="394" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="394" spans="1:10">
       <c r="A394" t="s">
         <v>401</v>
       </c>
@@ -14517,7 +14526,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="395" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="395" spans="1:10">
       <c r="A395" t="s">
         <v>402</v>
       </c>
@@ -14549,7 +14558,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="396" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="396" spans="1:10">
       <c r="A396" t="s">
         <v>403</v>
       </c>
@@ -14581,7 +14590,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="397" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="397" spans="1:10">
       <c r="A397" t="s">
         <v>404</v>
       </c>
@@ -14613,7 +14622,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="398" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="398" spans="1:10">
       <c r="A398" t="s">
         <v>405</v>
       </c>
@@ -14645,7 +14654,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="399" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="399" spans="1:10">
       <c r="A399" t="s">
         <v>406</v>
       </c>
@@ -14677,7 +14686,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="400" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="400" spans="1:10">
       <c r="A400" t="s">
         <v>407</v>
       </c>
@@ -14709,7 +14718,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="401" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="401" spans="1:10">
       <c r="A401" t="s">
         <v>408</v>
       </c>
@@ -14741,7 +14750,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="402" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="402" spans="1:10">
       <c r="A402" t="s">
         <v>409</v>
       </c>
@@ -14773,7 +14782,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="403" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="403" spans="1:10">
       <c r="A403" t="s">
         <v>410</v>
       </c>
@@ -14805,7 +14814,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="404" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="404" spans="1:10">
       <c r="A404" t="s">
         <v>411</v>
       </c>
@@ -14837,7 +14846,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="405" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="405" spans="1:10">
       <c r="A405" t="s">
         <v>412</v>
       </c>
@@ -14869,7 +14878,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="406" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="406" spans="1:10">
       <c r="A406" t="s">
         <v>413</v>
       </c>
@@ -14901,7 +14910,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="407" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="407" spans="1:10">
       <c r="A407" t="s">
         <v>414</v>
       </c>
@@ -14933,7 +14942,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="408" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="408" spans="1:10">
       <c r="A408" t="s">
         <v>415</v>
       </c>
@@ -14965,7 +14974,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="409" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="409" spans="1:10">
       <c r="A409" t="s">
         <v>416</v>
       </c>
@@ -14997,7 +15006,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="410" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="410" spans="1:10">
       <c r="A410" t="s">
         <v>417</v>
       </c>
@@ -15029,7 +15038,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="411" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="411" spans="1:10">
       <c r="A411" t="s">
         <v>418</v>
       </c>
@@ -15061,7 +15070,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="412" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="412" spans="1:10">
       <c r="A412" t="s">
         <v>419</v>
       </c>
@@ -15093,7 +15102,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="413" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="413" spans="1:10">
       <c r="A413" t="s">
         <v>420</v>
       </c>
@@ -15125,7 +15134,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="414" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="414" spans="1:10">
       <c r="A414" t="s">
         <v>421</v>
       </c>
@@ -15157,7 +15166,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="415" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="415" spans="1:10">
       <c r="A415" t="s">
         <v>422</v>
       </c>
@@ -15189,7 +15198,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="416" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="416" spans="1:10">
       <c r="A416" t="s">
         <v>423</v>
       </c>
@@ -15221,7 +15230,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="417" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="417" spans="1:10">
       <c r="A417" t="s">
         <v>424</v>
       </c>
@@ -15253,7 +15262,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="418" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="418" spans="1:10">
       <c r="A418" t="s">
         <v>425</v>
       </c>
@@ -15285,7 +15294,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="419" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="419" spans="1:10">
       <c r="A419" t="s">
         <v>426</v>
       </c>
@@ -15317,7 +15326,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="420" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="420" spans="1:10">
       <c r="A420" t="s">
         <v>427</v>
       </c>
@@ -15349,7 +15358,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="421" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="421" spans="1:10">
       <c r="A421" t="s">
         <v>428</v>
       </c>
@@ -15381,7 +15390,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="422" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="422" spans="1:10">
       <c r="A422" t="s">
         <v>429</v>
       </c>
@@ -15413,7 +15422,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="423" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="423" spans="1:10">
       <c r="A423" t="s">
         <v>430</v>
       </c>
@@ -15445,7 +15454,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="424" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="424" spans="1:10">
       <c r="A424" t="s">
         <v>431</v>
       </c>
@@ -15477,7 +15486,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="425" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="425" spans="1:10">
       <c r="A425" t="s">
         <v>432</v>
       </c>
@@ -15509,7 +15518,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="426" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="426" spans="1:10">
       <c r="A426" t="s">
         <v>433</v>
       </c>
@@ -15541,7 +15550,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="427" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="427" spans="1:10">
       <c r="A427" t="s">
         <v>434</v>
       </c>
@@ -15573,7 +15582,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="428" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="428" spans="1:10">
       <c r="A428" t="s">
         <v>435</v>
       </c>
@@ -15605,7 +15614,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="429" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="429" spans="1:10">
       <c r="A429" t="s">
         <v>436</v>
       </c>
@@ -15637,7 +15646,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="430" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="430" spans="1:10">
       <c r="A430" t="s">
         <v>437</v>
       </c>
@@ -15669,7 +15678,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="431" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="431" spans="1:10">
       <c r="A431" t="s">
         <v>438</v>
       </c>
@@ -15701,7 +15710,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="432" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="432" spans="1:10">
       <c r="A432" t="s">
         <v>439</v>
       </c>
@@ -15733,7 +15742,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="433" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="433" spans="1:10">
       <c r="A433" t="s">
         <v>440</v>
       </c>
@@ -15765,7 +15774,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="434" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="434" spans="1:10">
       <c r="A434" t="s">
         <v>441</v>
       </c>
@@ -15797,7 +15806,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="435" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="435" spans="1:10">
       <c r="A435" t="s">
         <v>442</v>
       </c>
@@ -15829,7 +15838,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="436" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="436" spans="1:10">
       <c r="A436" t="s">
         <v>443</v>
       </c>
@@ -15861,7 +15870,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="437" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="437" spans="1:10">
       <c r="A437" t="s">
         <v>444</v>
       </c>
@@ -15893,7 +15902,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="438" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="438" spans="1:10">
       <c r="A438" t="s">
         <v>445</v>
       </c>
@@ -15925,7 +15934,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="439" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="439" spans="1:10">
       <c r="A439" t="s">
         <v>446</v>
       </c>
@@ -15957,7 +15966,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="440" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="440" spans="1:10">
       <c r="A440" t="s">
         <v>447</v>
       </c>
@@ -15989,7 +15998,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="441" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="441" spans="1:10">
       <c r="A441" t="s">
         <v>448</v>
       </c>
@@ -16021,7 +16030,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="442" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="442" spans="1:10">
       <c r="A442" t="s">
         <v>449</v>
       </c>
@@ -16053,7 +16062,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="443" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="443" spans="1:10">
       <c r="A443" t="s">
         <v>450</v>
       </c>
@@ -16085,7 +16094,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="444" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="444" spans="1:10">
       <c r="A444" t="s">
         <v>451</v>
       </c>
@@ -16117,7 +16126,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="445" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="445" spans="1:10">
       <c r="A445" t="s">
         <v>452</v>
       </c>
@@ -16149,7 +16158,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="446" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="446" spans="1:10">
       <c r="A446" t="s">
         <v>453</v>
       </c>
@@ -16181,7 +16190,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="447" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="447" spans="1:10">
       <c r="A447" t="s">
         <v>454</v>
       </c>
@@ -16213,7 +16222,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="448" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="448" spans="1:10">
       <c r="A448" t="s">
         <v>455</v>
       </c>
@@ -16245,7 +16254,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="449" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="449" spans="1:10">
       <c r="A449" t="s">
         <v>456</v>
       </c>
@@ -16277,7 +16286,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="450" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="450" spans="1:10">
       <c r="A450" t="s">
         <v>457</v>
       </c>
@@ -16309,7 +16318,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="451" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="451" spans="1:10">
       <c r="A451" t="s">
         <v>458</v>
       </c>
@@ -16341,7 +16350,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="452" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="452" spans="1:10">
       <c r="A452" t="s">
         <v>459</v>
       </c>
@@ -16373,7 +16382,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="453" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="453" spans="1:10">
       <c r="A453" t="s">
         <v>460</v>
       </c>
@@ -16405,7 +16414,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="454" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="454" spans="1:10">
       <c r="A454" t="s">
         <v>461</v>
       </c>
@@ -16437,7 +16446,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="455" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="455" spans="1:10">
       <c r="A455" t="s">
         <v>462</v>
       </c>
@@ -16469,7 +16478,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="456" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="456" spans="1:10">
       <c r="A456" t="s">
         <v>463</v>
       </c>
@@ -16501,7 +16510,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="457" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="457" spans="1:10">
       <c r="A457" t="s">
         <v>464</v>
       </c>
@@ -16533,7 +16542,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="458" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="458" spans="1:10">
       <c r="A458" t="s">
         <v>465</v>
       </c>
@@ -16565,7 +16574,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="459" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="459" spans="1:10">
       <c r="A459" t="s">
         <v>466</v>
       </c>
@@ -16597,7 +16606,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="460" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="460" spans="1:10">
       <c r="A460" t="s">
         <v>467</v>
       </c>
@@ -16629,7 +16638,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="461" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="461" spans="1:10">
       <c r="A461" t="s">
         <v>468</v>
       </c>
@@ -16661,7 +16670,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="462" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="462" spans="1:10">
       <c r="A462" t="s">
         <v>469</v>
       </c>
@@ -16693,7 +16702,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="463" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="463" spans="1:10">
       <c r="A463" t="s">
         <v>470</v>
       </c>
@@ -16725,7 +16734,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="464" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="464" spans="1:10">
       <c r="A464" t="s">
         <v>471</v>
       </c>
@@ -16757,7 +16766,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="465" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="465" spans="1:10">
       <c r="A465" t="s">
         <v>472</v>
       </c>
@@ -16789,7 +16798,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="466" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="466" spans="1:10">
       <c r="A466" t="s">
         <v>473</v>
       </c>
@@ -16821,7 +16830,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="467" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="467" spans="1:10">
       <c r="A467" t="s">
         <v>474</v>
       </c>
@@ -16853,7 +16862,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="468" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="468" spans="1:10">
       <c r="A468" t="s">
         <v>475</v>
       </c>
@@ -16885,7 +16894,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="469" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="469" spans="1:10">
       <c r="A469" t="s">
         <v>476</v>
       </c>
@@ -16917,7 +16926,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="470" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="470" spans="1:10">
       <c r="A470" t="s">
         <v>477</v>
       </c>
@@ -16949,7 +16958,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="471" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="471" spans="1:10">
       <c r="A471" t="s">
         <v>478</v>
       </c>
@@ -16981,7 +16990,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="472" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="472" spans="1:10">
       <c r="A472" t="s">
         <v>479</v>
       </c>
@@ -17013,7 +17022,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="473" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="473" spans="1:10">
       <c r="A473" t="s">
         <v>480</v>
       </c>
@@ -17045,7 +17054,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="474" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="474" spans="1:10">
       <c r="A474" t="s">
         <v>481</v>
       </c>
@@ -17077,7 +17086,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="475" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="475" spans="1:10">
       <c r="A475" t="s">
         <v>482</v>
       </c>
@@ -17109,7 +17118,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="476" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="476" spans="1:10">
       <c r="A476" t="s">
         <v>483</v>
       </c>
@@ -17141,7 +17150,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="477" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="477" spans="1:10">
       <c r="A477" t="s">
         <v>484</v>
       </c>
@@ -17173,7 +17182,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="478" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="478" spans="1:10">
       <c r="A478" t="s">
         <v>485</v>
       </c>
@@ -17205,7 +17214,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="479" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="479" spans="1:10">
       <c r="A479" t="s">
         <v>486</v>
       </c>
@@ -17237,7 +17246,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="480" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="480" spans="1:10">
       <c r="A480" t="s">
         <v>487</v>
       </c>
@@ -17269,7 +17278,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="481" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="481" spans="1:10">
       <c r="A481" t="s">
         <v>488</v>
       </c>
@@ -17301,7 +17310,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="482" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="482" spans="1:10">
       <c r="A482" t="s">
         <v>489</v>
       </c>
@@ -17333,7 +17342,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="483" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="483" spans="1:10">
       <c r="A483" t="s">
         <v>490</v>
       </c>
@@ -17365,7 +17374,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="484" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="484" spans="1:10">
       <c r="A484" t="s">
         <v>491</v>
       </c>
@@ -17397,7 +17406,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="485" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="485" spans="1:10">
       <c r="A485" t="s">
         <v>492</v>
       </c>
@@ -17429,7 +17438,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="486" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="486" spans="1:10">
       <c r="A486" t="s">
         <v>493</v>
       </c>
@@ -17461,7 +17470,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="487" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="487" spans="1:10">
       <c r="A487" t="s">
         <v>494</v>
       </c>
@@ -17493,7 +17502,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="488" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="488" spans="1:10">
       <c r="A488" t="s">
         <v>495</v>
       </c>
@@ -17525,7 +17534,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="489" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="489" spans="1:10">
       <c r="A489" t="s">
         <v>496</v>
       </c>
@@ -17557,7 +17566,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="490" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="490" spans="1:10">
       <c r="A490" t="s">
         <v>497</v>
       </c>
@@ -17589,7 +17598,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="491" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="491" spans="1:10">
       <c r="A491" t="s">
         <v>498</v>
       </c>
@@ -17621,7 +17630,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="492" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="492" spans="1:10">
       <c r="A492" t="s">
         <v>499</v>
       </c>
@@ -17653,7 +17662,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="493" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="493" spans="1:10">
       <c r="A493" t="s">
         <v>500</v>
       </c>
@@ -17685,7 +17694,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="494" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="494" spans="1:10">
       <c r="A494" t="s">
         <v>501</v>
       </c>
@@ -17717,7 +17726,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="495" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="495" spans="1:10">
       <c r="A495" t="s">
         <v>502</v>
       </c>
@@ -17749,7 +17758,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="496" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="496" spans="1:10">
       <c r="A496" t="s">
         <v>503</v>
       </c>
@@ -17781,7 +17790,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="497" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="497" spans="1:10">
       <c r="A497" t="s">
         <v>504</v>
       </c>
@@ -17813,7 +17822,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="498" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="498" spans="1:10">
       <c r="A498" t="s">
         <v>505</v>
       </c>
@@ -17845,7 +17854,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="499" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="499" spans="1:10">
       <c r="A499" t="s">
         <v>506</v>
       </c>
@@ -17877,7 +17886,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="500" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="500" spans="1:10">
       <c r="A500" t="s">
         <v>507</v>
       </c>
@@ -17909,7 +17918,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="501" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="501" spans="1:10">
       <c r="A501" t="s">
         <v>508</v>
       </c>
@@ -17941,7 +17950,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="502" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="502" spans="1:10">
       <c r="A502" t="s">
         <v>509</v>
       </c>
@@ -17973,7 +17982,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="503" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="503" spans="1:10">
       <c r="A503" t="s">
         <v>510</v>
       </c>
@@ -18005,7 +18014,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="504" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="504" spans="1:10">
       <c r="A504" t="s">
         <v>511</v>
       </c>
@@ -18037,7 +18046,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="505" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="505" spans="1:10">
       <c r="A505" t="s">
         <v>512</v>
       </c>
@@ -18069,7 +18078,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="506" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="506" spans="1:10">
       <c r="A506" t="s">
         <v>513</v>
       </c>
@@ -18101,7 +18110,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="507" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="507" spans="1:10">
       <c r="A507" t="s">
         <v>514</v>
       </c>
@@ -18133,7 +18142,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="508" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="508" spans="1:10">
       <c r="A508" t="s">
         <v>515</v>
       </c>
@@ -18165,7 +18174,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="509" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="509" spans="1:10">
       <c r="A509" t="s">
         <v>516</v>
       </c>
@@ -18197,7 +18206,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="510" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="510" spans="1:10">
       <c r="A510" t="s">
         <v>517</v>
       </c>
@@ -18229,7 +18238,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="511" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="511" spans="1:10">
       <c r="A511" t="s">
         <v>518</v>
       </c>
@@ -18261,7 +18270,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="512" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="512" spans="1:10">
       <c r="A512" t="s">
         <v>519</v>
       </c>
@@ -18293,7 +18302,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="513" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="513" spans="1:10">
       <c r="A513" t="s">
         <v>520</v>
       </c>
@@ -18327,5 +18336,10 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>